<commit_message>
Updates to parameter work: Basically done, but waiting on email responses
</commit_message>
<xml_diff>
--- a/docs/notes/parametermusings/parameters.xlsx
+++ b/docs/notes/parametermusings/parameters.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23400" yWindow="7720" windowWidth="27520" windowHeight="18400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="15460" yWindow="2120" windowWidth="33520" windowHeight="24440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
     <sheet name="params" sheetId="1" r:id="rId2"/>
     <sheet name="papers_checked" sheetId="4" r:id="rId3"/>
-    <sheet name="scratch" sheetId="3" r:id="rId4"/>
+    <sheet name="HarpoleTilman2006" sheetId="5" r:id="rId4"/>
+    <sheet name="scratch" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="260">
   <si>
     <t>Parameter</t>
   </si>
@@ -114,9 +115,6 @@
     <t>Estimate_additional1</t>
   </si>
   <si>
-    <t>Estimate_additionalORrange</t>
-  </si>
-  <si>
     <t>Levine_HilleRisLambers_2009</t>
   </si>
   <si>
@@ -124,9 +122,6 @@
   </si>
   <si>
     <t>Gives seedbank survival rates for 10 spp (% survived, I assume for one year but hard to tell)</t>
-  </si>
-  <si>
-    <t>Godoy_Levine_2014</t>
   </si>
   <si>
     <t>per germinant seed production in the absence of competition</t>
@@ -234,9 +229,6 @@
 Search language=Auto  </t>
   </si>
   <si>
-    <t>Need to request ILL, may not be in language that I read: Coexistence in a variable and unpredictable habitat: The importance of the seed bank and contrasted regeneration niche for annual plants in temporary pools</t>
-  </si>
-  <si>
     <t>Descaps-Julien_Gonzalez_2005</t>
   </si>
   <si>
@@ -288,9 +280,6 @@
     <t>Gleeson_Tilman_1992</t>
   </si>
   <si>
-    <t>Worth looking into further … maybe:</t>
-  </si>
-  <si>
     <t>Tilman_etal_1997</t>
   </si>
   <si>
@@ -375,24 +364,9 @@
     <t>mass_after_46_days_growth</t>
   </si>
   <si>
-    <t>g_per_6ind</t>
-  </si>
-  <si>
     <t>Goldberg_&amp;_Fleetwood_1987</t>
   </si>
   <si>
-    <t>95CI of 51</t>
-  </si>
-  <si>
-    <t>95CI of 702</t>
-  </si>
-  <si>
-    <t>95CI of 139</t>
-  </si>
-  <si>
-    <t>95CI of 393</t>
-  </si>
-  <si>
     <t>pots_on_benches</t>
   </si>
   <si>
@@ -426,15 +400,9 @@
     <t>Dybzinski_&amp;_Tilman_2007</t>
   </si>
   <si>
-    <t>monocultures in the field (outside!)</t>
-  </si>
-  <si>
     <t>Rstar (nitrate)</t>
   </si>
   <si>
-    <t>0.05-0.4</t>
-  </si>
-  <si>
     <t>Rstar</t>
   </si>
   <si>
@@ -444,9 +412,6 @@
     <t>six grass spp under varying soil N</t>
   </si>
   <si>
-    <t>0.1-0.9</t>
-  </si>
-  <si>
     <t>nitrate</t>
   </si>
   <si>
@@ -471,12 +436,6 @@
     <t>g m-2</t>
   </si>
   <si>
-    <t>10-1000</t>
-  </si>
-  <si>
-    <t>see Figs 2-4; they also give the weight of each SEED Table 1) and they g per m2 of each spp that they seeded out (pg 307, last full paragraph on left side) so you could sort of estimate SEED -&gt; biomass if we wanted to.</t>
-  </si>
-  <si>
     <t>Rstar (P)</t>
   </si>
   <si>
@@ -489,18 +448,6 @@
     <t>Rstar (DIN)</t>
   </si>
   <si>
-    <t>3.07-14.8</t>
-  </si>
-  <si>
-    <t>44.3-87.6</t>
-  </si>
-  <si>
-    <t>11.25-19.81</t>
-  </si>
-  <si>
-    <t>9.9-12.5</t>
-  </si>
-  <si>
     <t>DIN</t>
   </si>
   <si>
@@ -510,9 +457,6 @@
     <t>percent water</t>
   </si>
   <si>
-    <t>micrograms per g</t>
-  </si>
-  <si>
     <t>Table 1</t>
   </si>
   <si>
@@ -525,21 +469,6 @@
     <t>ungrazed biomass (monoculture)</t>
   </si>
   <si>
-    <t>88.36-511.1</t>
-  </si>
-  <si>
-    <t>0.509-99.24</t>
-  </si>
-  <si>
-    <t>mixtures in the field (outside!)</t>
-  </si>
-  <si>
-    <t>Fig 2</t>
-  </si>
-  <si>
-    <t>overall seed masses also given per species and relative to each other, see top of pg 1149 (right side) for info on gram to seed conversion</t>
-  </si>
-  <si>
     <t>overview of Rstar papers</t>
   </si>
   <si>
@@ -552,12 +481,6 @@
     <t>six exotic herbs and six native herbs (some grasses)</t>
   </si>
   <si>
-    <t>3 to 20</t>
-  </si>
-  <si>
-    <t>mg N per kg soil</t>
-  </si>
-  <si>
     <t>monocultures in field</t>
   </si>
   <si>
@@ -565,13 +488,373 @@
   </si>
   <si>
     <t>Fig 2b</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>hulled seed mass</t>
+  </si>
+  <si>
+    <t>Table 1, also has error if wanted</t>
+  </si>
+  <si>
+    <t>mass of seed, I assume as rec'd from Prairie Restorations (Princeton, MN)</t>
+  </si>
+  <si>
+    <t>Schizachyrium scoparium</t>
+  </si>
+  <si>
+    <t>Andropogon gerardii</t>
+  </si>
+  <si>
+    <t>Panicum virgatum</t>
+  </si>
+  <si>
+    <t>Bouteloua gracilis</t>
+  </si>
+  <si>
+    <t>Buchloe dactyloides</t>
+  </si>
+  <si>
+    <t>Agropyron smithii</t>
+  </si>
+  <si>
+    <t>see Figs 2-4; they also give the g per m2 of each spp that they seeded out (pg 307, last full paragraph on left side) so you could sort of estimate SEED -&gt; biomass if we wanted to (but I do not see biomass -&gt; seed)</t>
+  </si>
+  <si>
+    <t>Estimate_additional_OR_range</t>
+  </si>
+  <si>
+    <t>estimated per seed mass</t>
+  </si>
+  <si>
+    <t>Avena barbata</t>
+  </si>
+  <si>
+    <t>Calandrinia ciliata</t>
+  </si>
+  <si>
+    <t>see top of pg 1149 (right side)</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>perennial</t>
+  </si>
+  <si>
+    <t>plant tissue death rate</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>imaginary</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>imaginary semi-arid</t>
+  </si>
+  <si>
+    <t>Cedar Creek</t>
+  </si>
+  <si>
+    <t>Los Olivos, California</t>
+  </si>
+  <si>
+    <t>Santa Ynez Valley, California</t>
+  </si>
+  <si>
+    <t>Kellog Bio Stn</t>
+  </si>
+  <si>
+    <t>Sedgewick, California</t>
+  </si>
+  <si>
+    <t>seed mass</t>
+  </si>
+  <si>
+    <t>Table 1, no error</t>
+  </si>
+  <si>
+    <t>g_per_ind</t>
+  </si>
+  <si>
+    <t>Table 1, SE given if wanted</t>
+  </si>
+  <si>
+    <t>Everard_etal_2010</t>
+  </si>
+  <si>
+    <t>water input rate</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>average mean rainfall</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>highly variable; start of Model Parameterization with California Grassland Data</t>
+  </si>
+  <si>
+    <t>b_i</t>
+  </si>
+  <si>
+    <t>day-1</t>
+  </si>
+  <si>
+    <t>mm day-1</t>
+  </si>
+  <si>
+    <t>mm yr-1</t>
+  </si>
+  <si>
+    <t>On 1. April.2016</t>
+  </si>
+  <si>
+    <t>I got a lot of good ideas for papers to look at from emails I sent out. See parameters_rstar.rtf for more.</t>
+  </si>
+  <si>
+    <t>I am only using exponents: so g per day would be g day-1</t>
+  </si>
+  <si>
+    <t>I also tried to divide out to ONE individual whenever possible.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I tried to standarize how I write </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UNITS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> today. </t>
+    </r>
+  </si>
+  <si>
+    <t>mgN kg-1 of soil</t>
+  </si>
+  <si>
+    <t>micrograms g-1</t>
+  </si>
+  <si>
+    <t>Table 1; 95CI of 51</t>
+  </si>
+  <si>
+    <t>Table 1; 95CI of 139</t>
+  </si>
+  <si>
+    <t>Table 1; 95CI of 393</t>
+  </si>
+  <si>
+    <t>Table 1; 95CI of 702</t>
+  </si>
+  <si>
+    <t>a1: active uptake efficiency (see eqn 5)</t>
+  </si>
+  <si>
+    <t>a1: active uptake efficiency  (see eqn 5)</t>
+  </si>
+  <si>
+    <t>a2: nonlinearity of active uptake efficiency with respect to soil moisture  (see eqn 5)</t>
+  </si>
+  <si>
+    <t>dimensionless</t>
+  </si>
+  <si>
+    <t>model with field parameters</t>
+  </si>
+  <si>
+    <t>Harpole_&amp;_Tilman_2006</t>
+  </si>
+  <si>
+    <t>Cedar Creek and Konza</t>
+  </si>
+  <si>
+    <t>mg kg-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achillea millefolium </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agastache foeniculum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agropyron repens </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agrostis scabra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Andropogon gerardii </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anemone cylindrica </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asclepias syriaca </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asclepias tuberosa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asclepias verticillata </t>
+  </si>
+  <si>
+    <t>Aster azureus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aster ericoides </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bouteloua curtipendula </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calamovilfa longifolia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coreopsis palmata </t>
+  </si>
+  <si>
+    <t>Koeleria cristata</t>
+  </si>
+  <si>
+    <t>Liatris aspera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panicum virgatum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penstemon grandiflorus </t>
+  </si>
+  <si>
+    <t>Poa pratensis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potentilla arguta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rudbeckia serotina </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schizachyrium scoparium </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solidago nemoralis </t>
+  </si>
+  <si>
+    <t>Solidago rigida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Solidago speciosa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorghastrum nutans </t>
+  </si>
+  <si>
+    <t>Stipa spartea</t>
+  </si>
+  <si>
+    <t>Table 1; SD given</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>twenty seven forbs and grasses (see tab for full list)</t>
+  </si>
+  <si>
+    <t>HilleRisLambers_etal_2004</t>
+  </si>
+  <si>
+    <t>Compares yield exponents (as in over and underyielding stuff) at Cedar Creek with lots of stuff</t>
+  </si>
+  <si>
+    <t>Rstar, some biomass data, Cedar Creek -- I think we have these values already; paper compares yield exponents (as in over and underyielding stuff)  with lots of stuff</t>
+  </si>
+  <si>
+    <t>Seabloom_etal_2003</t>
+  </si>
+  <si>
+    <t>Bromus hordeaceus</t>
+  </si>
+  <si>
+    <t>Bromus madritensis</t>
+  </si>
+  <si>
+    <t>Hordeum murinum</t>
+  </si>
+  <si>
+    <t>seeds_per_plant</t>
+  </si>
+  <si>
+    <t>seed production per plant in plots with annual or perennial species</t>
+  </si>
+  <si>
+    <t>Table 1: SE also given, range is production in perennial plots (lower values) annual plots</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sedgewick weather data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> only goes to 2011: http://www.wrcc.dri.edu/weather/ucse.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Some notes from today:</t>
+  </si>
+  <si>
+    <t>Godoy &amp; Levine 2014 (Ecology) do NOT give biomass (though they have it in some way based on Fig. 1).</t>
+  </si>
+  <si>
+    <t>Godoy_Levine_2014Ecology</t>
+  </si>
+  <si>
+    <t>Sent emails to Eric Seabloom and Janneke HilleRisLambers to see if they have data to estimate seed production per unit biomass.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -610,6 +893,32 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -628,7 +937,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="159">
+  <cellStyleXfs count="319">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -788,15 +1097,179 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="159">
+  <cellStyles count="319">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -876,6 +1349,86 @@
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -955,6 +1508,86 @@
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1284,21 +1917,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1314,48 +1947,86 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:1" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>96</v>
+      <c r="A12" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
-        <v>87</v>
+      <c r="A23" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="B24" t="s">
-        <v>69</v>
-      </c>
+      <c r="A24" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1370,29 +2041,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="53.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="54.6640625" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1401,7 +2075,7 @@
         <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
@@ -1413,15 +2087,18 @@
         <v>2</v>
       </c>
       <c r="J1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D2">
         <v>0.5</v>
@@ -1438,10 +2115,13 @@
       <c r="I2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="J2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1458,10 +2138,13 @@
       <c r="I3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="J3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -1481,10 +2164,13 @@
       <c r="I4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="J4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -1501,10 +2187,13 @@
       <c r="I5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="J5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -1521,10 +2210,13 @@
       <c r="I6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
         <v>24</v>
@@ -1544,10 +2236,13 @@
       <c r="I7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1570,10 +2265,13 @@
       <c r="I8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="J8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1590,8 +2288,11 @@
       <c r="I9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="J9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1610,8 +2311,11 @@
       <c r="I10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1633,8 +2337,11 @@
       <c r="I11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="J11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1642,7 +2349,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>0.4</v>
@@ -1659,8 +2366,11 @@
       <c r="I12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="J12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1679,8 +2389,11 @@
       <c r="I13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="J13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1699,8 +2412,11 @@
       <c r="I14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="J14" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1719,8 +2435,11 @@
       <c r="I15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="J15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1739,842 +2458,1646 @@
       <c r="I16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="J16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="I17" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>1993</v>
       </c>
       <c r="G18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19">
         <v>7670</v>
       </c>
       <c r="G19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I19" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D20">
         <v>20759</v>
       </c>
       <c r="G20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I20" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21">
         <v>23</v>
       </c>
       <c r="G21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I21" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22">
         <v>248</v>
       </c>
       <c r="G22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I22" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J22" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D23">
         <v>582</v>
       </c>
       <c r="G23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I23" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24">
         <v>0.32</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I24" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D25">
         <v>0.21</v>
       </c>
       <c r="G25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J25" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>0.12</v>
       </c>
       <c r="G26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I26" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D27">
         <v>0.12</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I27" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D28">
         <v>0.45</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I28" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D29">
         <v>0.33</v>
       </c>
       <c r="G29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I29" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D30">
         <v>0.02</v>
       </c>
       <c r="G30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I30" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D31">
         <v>0.54</v>
       </c>
       <c r="G31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I31" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J31" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D32">
         <v>0.43</v>
       </c>
       <c r="G32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I32" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J32" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+        <v>181</v>
+      </c>
+      <c r="K32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D33">
         <v>0.32</v>
       </c>
       <c r="G33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I33" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J33" t="s">
+        <v>181</v>
+      </c>
+      <c r="K33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D34">
         <v>0.2</v>
       </c>
       <c r="G34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I34" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J34" t="s">
+        <v>181</v>
+      </c>
+      <c r="K34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" t="s">
-        <v>61</v>
-      </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D35">
         <v>0.51</v>
       </c>
       <c r="G35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I35" t="s">
-        <v>34</v>
+        <v>258</v>
       </c>
       <c r="J35" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" t="s">
+        <v>181</v>
+      </c>
+      <c r="K35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" s="5" customFormat="1">
+      <c r="A36" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="5">
+        <f>0.034/6</f>
+        <v>5.6666666666666671E-3</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I36" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D36">
-        <v>34</v>
-      </c>
-      <c r="G36" t="s">
-        <v>116</v>
-      </c>
-      <c r="H36" t="s">
-        <v>122</v>
-      </c>
-      <c r="I36" t="s">
-        <v>117</v>
-      </c>
-      <c r="J36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="J36" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" s="5" customFormat="1">
+      <c r="A37" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D37">
-        <v>431</v>
-      </c>
-      <c r="G37" t="s">
-        <v>116</v>
-      </c>
-      <c r="H37" t="s">
-        <v>122</v>
-      </c>
-      <c r="I37" t="s">
-        <v>117</v>
-      </c>
-      <c r="J37" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="C37" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="5">
+        <f>0.431/6</f>
+        <v>7.1833333333333332E-2</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="H37" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D38">
-        <v>1128</v>
-      </c>
-      <c r="G38" t="s">
-        <v>116</v>
-      </c>
-      <c r="H38" t="s">
-        <v>122</v>
-      </c>
-      <c r="I38" t="s">
-        <v>117</v>
-      </c>
-      <c r="J38" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" t="s">
-        <v>115</v>
-      </c>
-      <c r="C39" t="s">
-        <v>114</v>
-      </c>
-      <c r="D39">
-        <v>1647</v>
-      </c>
-      <c r="G39" t="s">
-        <v>116</v>
-      </c>
-      <c r="H39" t="s">
-        <v>122</v>
-      </c>
-      <c r="I39" t="s">
-        <v>117</v>
-      </c>
-      <c r="J39" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" t="s">
+      <c r="I37" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="5" customFormat="1">
+      <c r="A38" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="5">
+        <f>1.128/6</f>
+        <v>0.18799999999999997</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="5" customFormat="1">
+      <c r="A39" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="5">
+        <f>1.647/6</f>
+        <v>0.27450000000000002</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" s="5" customFormat="1">
+      <c r="A40" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="5">
+        <f>0.65/10</f>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K40" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" s="5" customFormat="1">
+      <c r="A41" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="5">
+        <f>0.14/10</f>
+        <v>1.4000000000000002E-2</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" s="5" customFormat="1">
+      <c r="A42" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="5">
+        <f>40/10</f>
+        <v>4</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="5" customFormat="1">
+      <c r="A43" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="5">
+        <f>34/10</f>
+        <v>3.4</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44">
+        <v>0.05</v>
+      </c>
+      <c r="F44">
+        <v>0.4</v>
+      </c>
+      <c r="G44" t="s">
+        <v>128</v>
+      </c>
+      <c r="H44" t="s">
+        <v>151</v>
+      </c>
+      <c r="I44" t="s">
+        <v>123</v>
+      </c>
+      <c r="J44" t="s">
+        <v>177</v>
+      </c>
+      <c r="K44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>126</v>
+      </c>
+      <c r="B45" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45">
+        <v>0.1</v>
+      </c>
+      <c r="F45">
+        <v>0.9</v>
+      </c>
+      <c r="G45" t="s">
+        <v>129</v>
+      </c>
+      <c r="H45" t="s">
+        <v>151</v>
+      </c>
+      <c r="I45" t="s">
+        <v>123</v>
+      </c>
+      <c r="J45" t="s">
+        <v>177</v>
+      </c>
+      <c r="K45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" t="s">
         <v>134</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D46">
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>1000</v>
+      </c>
+      <c r="G46" t="s">
+        <v>135</v>
+      </c>
+      <c r="H46" t="s">
+        <v>151</v>
+      </c>
+      <c r="I46" t="s">
+        <v>123</v>
+      </c>
+      <c r="J46" t="s">
+        <v>177</v>
+      </c>
+      <c r="K46" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" t="s">
+        <v>192</v>
+      </c>
+      <c r="C47" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47">
+        <v>3.27</v>
+      </c>
+      <c r="G47" t="s">
+        <v>154</v>
+      </c>
+      <c r="H47" t="s">
+        <v>157</v>
+      </c>
+      <c r="I47" t="s">
+        <v>123</v>
+      </c>
+      <c r="J47" t="s">
+        <v>177</v>
+      </c>
+      <c r="K47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" t="s">
+        <v>155</v>
+      </c>
+      <c r="B48" t="s">
+        <v>192</v>
+      </c>
+      <c r="C48" t="s">
+        <v>159</v>
+      </c>
+      <c r="D48">
+        <v>1.7</v>
+      </c>
+      <c r="G48" t="s">
+        <v>154</v>
+      </c>
+      <c r="H48" t="s">
+        <v>157</v>
+      </c>
+      <c r="I48" t="s">
+        <v>123</v>
+      </c>
+      <c r="J48" t="s">
+        <v>177</v>
+      </c>
+      <c r="K48" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49">
+        <v>1.57</v>
+      </c>
+      <c r="G49" t="s">
+        <v>154</v>
+      </c>
+      <c r="H49" t="s">
+        <v>157</v>
+      </c>
+      <c r="I49" t="s">
+        <v>123</v>
+      </c>
+      <c r="J49" t="s">
+        <v>177</v>
+      </c>
+      <c r="K49" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" t="s">
+        <v>192</v>
+      </c>
+      <c r="C50" t="s">
+        <v>160</v>
+      </c>
+      <c r="D50">
+        <v>1.45</v>
+      </c>
+      <c r="G50" t="s">
+        <v>154</v>
+      </c>
+      <c r="H50" t="s">
+        <v>157</v>
+      </c>
+      <c r="I50" t="s">
+        <v>123</v>
+      </c>
+      <c r="J50" t="s">
+        <v>177</v>
+      </c>
+      <c r="K50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" t="s">
+        <v>192</v>
+      </c>
+      <c r="C51" t="s">
+        <v>158</v>
+      </c>
+      <c r="D51">
+        <v>0.4</v>
+      </c>
+      <c r="G51" t="s">
+        <v>154</v>
+      </c>
+      <c r="H51" t="s">
+        <v>157</v>
+      </c>
+      <c r="I51" t="s">
+        <v>123</v>
+      </c>
+      <c r="J51" t="s">
+        <v>177</v>
+      </c>
+      <c r="K51" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" t="s">
+        <v>155</v>
+      </c>
+      <c r="B52" t="s">
+        <v>192</v>
+      </c>
+      <c r="C52" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52">
+        <v>0.21</v>
+      </c>
+      <c r="G52" t="s">
+        <v>154</v>
+      </c>
+      <c r="H52" t="s">
+        <v>157</v>
+      </c>
+      <c r="I52" t="s">
+        <v>123</v>
+      </c>
+      <c r="J52" t="s">
+        <v>177</v>
+      </c>
+      <c r="K52" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53">
+        <v>3.07</v>
+      </c>
+      <c r="F53">
+        <v>14.8</v>
+      </c>
+      <c r="G53" t="s">
+        <v>140</v>
+      </c>
+      <c r="H53" t="s">
+        <v>151</v>
+      </c>
+      <c r="I53" t="s">
+        <v>144</v>
+      </c>
+      <c r="J53" t="s">
+        <v>179</v>
+      </c>
+      <c r="K53" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" t="s">
+        <v>126</v>
+      </c>
+      <c r="B54" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54">
+        <v>44.3</v>
+      </c>
+      <c r="F54">
+        <v>87.6</v>
+      </c>
+      <c r="G54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H54" t="s">
+        <v>151</v>
+      </c>
+      <c r="I54" t="s">
+        <v>144</v>
+      </c>
+      <c r="J54" t="s">
+        <v>179</v>
+      </c>
+      <c r="K54" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" t="s">
         <v>136</v>
       </c>
-      <c r="C40" t="s">
+      <c r="B55" t="s">
+        <v>125</v>
+      </c>
+      <c r="C55" t="s">
         <v>138</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D55">
+        <v>11.25</v>
+      </c>
+      <c r="F55">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="G55" t="s">
+        <v>202</v>
+      </c>
+      <c r="H55" t="s">
+        <v>151</v>
+      </c>
+      <c r="I55" t="s">
+        <v>144</v>
+      </c>
+      <c r="J55" t="s">
+        <v>179</v>
+      </c>
+      <c r="K55" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" t="s">
+        <v>125</v>
+      </c>
+      <c r="C56" t="s">
+        <v>138</v>
+      </c>
+      <c r="D56">
+        <v>9.9</v>
+      </c>
+      <c r="F56">
+        <v>12.5</v>
+      </c>
+      <c r="G56" t="s">
+        <v>142</v>
+      </c>
+      <c r="H56" t="s">
+        <v>151</v>
+      </c>
+      <c r="I56" t="s">
+        <v>144</v>
+      </c>
+      <c r="J56" t="s">
+        <v>179</v>
+      </c>
+      <c r="K56" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" t="s">
+        <v>146</v>
+      </c>
+      <c r="B57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D57">
+        <v>88.36</v>
+      </c>
+      <c r="F57">
+        <v>511.1</v>
+      </c>
+      <c r="G57" t="s">
         <v>135</v>
       </c>
-      <c r="G40" t="s">
-        <v>140</v>
-      </c>
-      <c r="H40" t="s">
-        <v>133</v>
-      </c>
-      <c r="I40" t="s">
+      <c r="H57" t="s">
+        <v>151</v>
+      </c>
+      <c r="I57" t="s">
+        <v>144</v>
+      </c>
+      <c r="J57" t="s">
+        <v>179</v>
+      </c>
+      <c r="K57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58" t="s">
         <v>132</v>
       </c>
-      <c r="J40" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" t="s">
-        <v>137</v>
-      </c>
-      <c r="B41" t="s">
-        <v>136</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="C58" t="s">
         <v>138</v>
       </c>
-      <c r="D41" t="s">
-        <v>139</v>
-      </c>
-      <c r="G41" t="s">
-        <v>141</v>
-      </c>
-      <c r="H41" t="s">
-        <v>133</v>
-      </c>
-      <c r="I41" t="s">
-        <v>132</v>
-      </c>
-      <c r="J41" t="s">
+      <c r="D58">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F58">
+        <v>99.24</v>
+      </c>
+      <c r="G58" t="s">
+        <v>135</v>
+      </c>
+      <c r="H58" t="s">
+        <v>151</v>
+      </c>
+      <c r="I58" t="s">
+        <v>144</v>
+      </c>
+      <c r="J58" t="s">
+        <v>179</v>
+      </c>
+      <c r="K58" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
-      <c r="A42" t="s">
-        <v>145</v>
-      </c>
-      <c r="B42" t="s">
+    <row r="59" spans="1:11">
+      <c r="A59" t="s">
+        <v>166</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" t="s">
+        <v>167</v>
+      </c>
+      <c r="D59">
+        <f>(15/119)*1000</f>
+        <v>126.05042016806722</v>
+      </c>
+      <c r="G59" t="s">
+        <v>154</v>
+      </c>
+      <c r="I59" t="s">
         <v>144</v>
       </c>
-      <c r="C42" t="s">
-        <v>146</v>
-      </c>
-      <c r="D42" t="s">
-        <v>148</v>
-      </c>
-      <c r="G42" t="s">
-        <v>147</v>
-      </c>
-      <c r="H42" t="s">
-        <v>133</v>
-      </c>
-      <c r="I42" t="s">
-        <v>132</v>
-      </c>
-      <c r="J42" t="s">
+      <c r="J59" t="s">
+        <v>179</v>
+      </c>
+      <c r="K59" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C60" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60">
+        <f>(15/2822)*1000</f>
+        <v>5.3153791637136782</v>
+      </c>
+      <c r="G60" t="s">
+        <v>154</v>
+      </c>
+      <c r="I60" t="s">
+        <v>144</v>
+      </c>
+      <c r="J60" t="s">
+        <v>179</v>
+      </c>
+      <c r="K60" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" t="s">
+      <c r="B61" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" t="s">
+        <v>150</v>
+      </c>
+      <c r="D61" s="4">
+        <v>3</v>
+      </c>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4">
+        <v>20</v>
+      </c>
+      <c r="G61" t="s">
+        <v>201</v>
+      </c>
+      <c r="H61" t="s">
+        <v>151</v>
+      </c>
+      <c r="I61" t="s">
+        <v>152</v>
+      </c>
+      <c r="J61" t="s">
+        <v>178</v>
+      </c>
+      <c r="K61" t="s">
         <v>153</v>
       </c>
-      <c r="B43" t="s">
-        <v>136</v>
-      </c>
-      <c r="C43" t="s">
-        <v>152</v>
-      </c>
-      <c r="D43" t="s">
-        <v>154</v>
-      </c>
-      <c r="G43" t="s">
-        <v>158</v>
-      </c>
-      <c r="H43" t="s">
-        <v>133</v>
-      </c>
-      <c r="I43" t="s">
-        <v>163</v>
-      </c>
-      <c r="J43" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" t="s">
-        <v>137</v>
-      </c>
-      <c r="B44" t="s">
-        <v>136</v>
-      </c>
-      <c r="C44" t="s">
-        <v>152</v>
-      </c>
-      <c r="D44" t="s">
-        <v>155</v>
-      </c>
-      <c r="G44" t="s">
-        <v>159</v>
-      </c>
-      <c r="H44" t="s">
-        <v>133</v>
-      </c>
-      <c r="I44" t="s">
-        <v>163</v>
-      </c>
-      <c r="J44" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" t="s">
-        <v>150</v>
-      </c>
-      <c r="B45" t="s">
-        <v>136</v>
-      </c>
-      <c r="C45" t="s">
-        <v>152</v>
-      </c>
-      <c r="D45" t="s">
-        <v>156</v>
-      </c>
-      <c r="G45" t="s">
-        <v>161</v>
-      </c>
-      <c r="H45" t="s">
-        <v>133</v>
-      </c>
-      <c r="I45" t="s">
-        <v>163</v>
-      </c>
-      <c r="J45" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" t="s">
+    </row>
+    <row r="62" spans="1:11" s="5" customFormat="1">
+      <c r="A62" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" s="7">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K62" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="5" customFormat="1">
+      <c r="A63" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K63" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" t="s">
+        <v>188</v>
+      </c>
+      <c r="D64" s="4">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="G64" t="s">
+        <v>194</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I64" t="s">
+        <v>186</v>
+      </c>
+      <c r="J64" t="s">
+        <v>175</v>
+      </c>
+      <c r="K64" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" t="s">
+        <v>207</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D65" s="4">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="G65" t="s">
+        <v>194</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I65" t="s">
+        <v>186</v>
+      </c>
+      <c r="J65" t="s">
+        <v>175</v>
+      </c>
+      <c r="K65" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D66" s="4">
+        <v>37.75</v>
+      </c>
+      <c r="G66" t="s">
+        <v>194</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I66" t="s">
+        <v>186</v>
+      </c>
+      <c r="J66" t="s">
+        <v>175</v>
+      </c>
+      <c r="K66" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" t="s">
+        <v>209</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D67" s="4">
+        <v>-9.98</v>
+      </c>
+      <c r="G67" t="s">
+        <v>210</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I67" t="s">
+        <v>186</v>
+      </c>
+      <c r="J67" t="s">
+        <v>175</v>
+      </c>
+      <c r="K67" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" t="s">
+        <v>209</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="G68" t="s">
+        <v>210</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I68" t="s">
+        <v>186</v>
+      </c>
+      <c r="J68" t="s">
+        <v>175</v>
+      </c>
+      <c r="K68" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" t="s">
+        <v>189</v>
+      </c>
+      <c r="B69" t="s">
+        <v>190</v>
+      </c>
+      <c r="C69" t="s">
+        <v>188</v>
+      </c>
+      <c r="D69">
+        <v>506</v>
+      </c>
+      <c r="G69" t="s">
+        <v>195</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I69" t="s">
+        <v>186</v>
+      </c>
+      <c r="J69" t="s">
+        <v>175</v>
+      </c>
+      <c r="K69" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" t="s">
+        <v>124</v>
+      </c>
+      <c r="B70" t="s">
+        <v>125</v>
+      </c>
+      <c r="C70" t="s">
+        <v>244</v>
+      </c>
+      <c r="D70">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F70">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="G70" t="s">
+        <v>214</v>
+      </c>
+      <c r="H70" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B46" t="s">
-        <v>136</v>
-      </c>
-      <c r="C46" t="s">
-        <v>152</v>
-      </c>
-      <c r="D46" t="s">
-        <v>157</v>
-      </c>
-      <c r="G46" t="s">
-        <v>160</v>
-      </c>
-      <c r="H46" t="s">
-        <v>133</v>
-      </c>
-      <c r="I46" t="s">
-        <v>163</v>
-      </c>
-      <c r="J46" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" t="s">
-        <v>165</v>
-      </c>
-      <c r="B47" t="s">
-        <v>144</v>
-      </c>
-      <c r="C47" t="s">
-        <v>152</v>
-      </c>
-      <c r="D47" t="s">
-        <v>166</v>
-      </c>
-      <c r="G47" t="s">
-        <v>147</v>
-      </c>
-      <c r="H47" t="s">
-        <v>133</v>
-      </c>
-      <c r="I47" t="s">
-        <v>163</v>
-      </c>
-      <c r="J47" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" t="s">
-        <v>164</v>
-      </c>
-      <c r="B48" t="s">
-        <v>144</v>
-      </c>
-      <c r="C48" t="s">
-        <v>152</v>
-      </c>
-      <c r="D48" t="s">
-        <v>167</v>
-      </c>
-      <c r="G48" t="s">
-        <v>147</v>
-      </c>
-      <c r="H48" t="s">
-        <v>168</v>
-      </c>
-      <c r="I48" t="s">
-        <v>163</v>
-      </c>
-      <c r="J48" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49" t="s">
-        <v>170</v>
-      </c>
-      <c r="C49" t="s">
-        <v>152</v>
-      </c>
-      <c r="G49" t="s">
-        <v>147</v>
-      </c>
-      <c r="H49" t="s">
-        <v>133</v>
-      </c>
-      <c r="I49" t="s">
-        <v>163</v>
-      </c>
-      <c r="J49" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" t="s">
-        <v>173</v>
-      </c>
-      <c r="B50" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" t="s">
-        <v>174</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G50" t="s">
-        <v>176</v>
-      </c>
-      <c r="H50" t="s">
-        <v>177</v>
-      </c>
-      <c r="I50" t="s">
-        <v>178</v>
-      </c>
-      <c r="J50" t="s">
-        <v>179</v>
-      </c>
+      <c r="I70" t="s">
+        <v>212</v>
+      </c>
+      <c r="J70" t="s">
+        <v>213</v>
+      </c>
+      <c r="K70" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>253</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D71">
+        <v>32.049999999999997</v>
+      </c>
+      <c r="F71">
+        <v>111.33</v>
+      </c>
+      <c r="G71" t="s">
+        <v>252</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I71" t="s">
+        <v>248</v>
+      </c>
+      <c r="J71" t="s">
+        <v>181</v>
+      </c>
+      <c r="K71" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" t="s">
+        <v>253</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D72">
+        <v>57.07</v>
+      </c>
+      <c r="F72">
+        <v>176.34</v>
+      </c>
+      <c r="G72" t="s">
+        <v>252</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I72" t="s">
+        <v>248</v>
+      </c>
+      <c r="J72" t="s">
+        <v>181</v>
+      </c>
+      <c r="K72" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" t="s">
+        <v>253</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D73">
+        <v>45.82</v>
+      </c>
+      <c r="F73">
+        <v>95.3</v>
+      </c>
+      <c r="G73" t="s">
+        <v>252</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I73" t="s">
+        <v>248</v>
+      </c>
+      <c r="J73" t="s">
+        <v>181</v>
+      </c>
+      <c r="K73" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="6"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2589,17 +4112,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
@@ -2607,7 +4131,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2624,163 +4148,174 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
         <v>72</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" t="s">
         <v>76</v>
-      </c>
-      <c r="B4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" t="s">
         <v>77</v>
-      </c>
-      <c r="F5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
         <v>82</v>
       </c>
-      <c r="B6" t="s">
-        <v>85</v>
-      </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="F17" t="s">
-        <v>172</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>247</v>
+      </c>
+      <c r="F18" t="s">
+        <v>245</v>
+      </c>
+      <c r="G18" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2795,6 +4330,257 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30:G56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B3">
+        <v>0.183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4">
+        <v>0.38700000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5">
+        <v>0.65900000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6">
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9">
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10">
+        <v>0.24199999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B11">
+        <v>0.51500000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B12">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B13">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14">
+        <v>0.29699999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15">
+        <v>0.161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16">
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B17">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18">
+        <v>0.38100000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B19">
+        <v>0.32100000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B20">
+        <v>0.22600000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B21">
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22">
+        <v>0.52100000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B23">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B24">
+        <v>0.13300000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B25">
+        <v>6.9000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B26">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B27">
+        <v>0.17899999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B28">
+        <v>0.44</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="G30:G56">
+    <sortCondition ref="G30:G56"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Progress on adding in the parameter data from Janneke
Not quite done yet ....
</commit_message>
<xml_diff>
--- a/docs/notes/parametermusings/parameters.xlsx
+++ b/docs/notes/parametermusings/parameters.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15460" yWindow="2120" windowWidth="33520" windowHeight="24440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="21160" yWindow="280" windowWidth="30040" windowHeight="20760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
     <sheet name="params" sheetId="1" r:id="rId2"/>
     <sheet name="papers_checked" sheetId="4" r:id="rId3"/>
-    <sheet name="HarpoleTilman2006" sheetId="5" r:id="rId4"/>
-    <sheet name="scratch" sheetId="3" r:id="rId5"/>
+    <sheet name="HilleRisLambers2010_data" sheetId="6" r:id="rId4"/>
+    <sheet name="HarpoleTilman2006" sheetId="5" r:id="rId5"/>
+    <sheet name="scratch" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="275">
   <si>
     <t>Parameter</t>
   </si>
@@ -535,9 +536,6 @@
     <t>Calandrinia ciliata</t>
   </si>
   <si>
-    <t>see top of pg 1149 (right side)</t>
-  </si>
-  <si>
     <t>annual</t>
   </si>
   <si>
@@ -560,9 +558,6 @@
   </si>
   <si>
     <t>Cedar Creek</t>
-  </si>
-  <si>
-    <t>Los Olivos, California</t>
   </si>
   <si>
     <t>Santa Ynez Valley, California</t>
@@ -848,6 +843,57 @@
   </si>
   <si>
     <t>Sent emails to Eric Seabloom and Janneke HilleRisLambers to see if they have data to estimate seed production per unit biomass.</t>
+  </si>
+  <si>
+    <t>Amsinckia menziesii</t>
+  </si>
+  <si>
+    <t>Clarkia purpurea</t>
+  </si>
+  <si>
+    <t>Lamarckia aurea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polypogon monspeliensis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vulpia microstachys </t>
+  </si>
+  <si>
+    <t>Vulpia myuros</t>
+  </si>
+  <si>
+    <t>Vulpia octoflora</t>
+  </si>
+  <si>
+    <t>Estimate_Raw</t>
+  </si>
+  <si>
+    <t>from DataScript_CAData_09152016</t>
+  </si>
+  <si>
+    <t>Data from HilleRisLambers_etal_2010</t>
+  </si>
+  <si>
+    <t>micrograms g-1 P</t>
+  </si>
+  <si>
+    <t>micrograms g-1 N</t>
+  </si>
+  <si>
+    <t>from SeedDat.csv, 2005 data</t>
+  </si>
+  <si>
+    <t>relative abundance (out of 1)</t>
+  </si>
+  <si>
+    <t>from DataScript_CAData_09152016 (mrelabun)</t>
+  </si>
+  <si>
+    <t>mixture plots in field</t>
+  </si>
+  <si>
+    <t>relative abundance (biomass across mixture plots)</t>
   </si>
 </sst>
 </file>
@@ -920,12 +966,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -937,7 +989,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="319">
+  <cellStyleXfs count="455">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1257,8 +1309,144 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1268,8 +1456,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="319">
+  <cellStyles count="455">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1429,6 +1621,74 @@
     <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="422" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="424" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="426" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="428" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="430" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="432" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="434" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="436" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1588,6 +1848,74 @@
     <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="421" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="423" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="425" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="427" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="429" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="431" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="433" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="435" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="437" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="439" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="441" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="443" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="445" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="447" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="449" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="451" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="453" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1982,47 +2310,47 @@
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="B19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="33" spans="1:1">
@@ -2041,11 +2369,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2087,7 +2415,7 @@
         <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
@@ -2116,7 +2444,7 @@
         <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2139,7 +2467,7 @@
         <v>9</v>
       </c>
       <c r="J3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2165,7 +2493,7 @@
         <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2188,7 +2516,7 @@
         <v>9</v>
       </c>
       <c r="J5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2211,7 +2539,7 @@
         <v>9</v>
       </c>
       <c r="J6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2237,7 +2565,7 @@
         <v>9</v>
       </c>
       <c r="J7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -2266,7 +2594,7 @@
         <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2289,7 +2617,7 @@
         <v>9</v>
       </c>
       <c r="J9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2312,7 +2640,7 @@
         <v>9</v>
       </c>
       <c r="J10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2338,7 +2666,7 @@
         <v>9</v>
       </c>
       <c r="J11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2367,7 +2695,7 @@
         <v>9</v>
       </c>
       <c r="J12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2390,7 +2718,7 @@
         <v>9</v>
       </c>
       <c r="J13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2413,7 +2741,7 @@
         <v>9</v>
       </c>
       <c r="J14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2436,7 +2764,7 @@
         <v>9</v>
       </c>
       <c r="J15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2459,7 +2787,7 @@
         <v>9</v>
       </c>
       <c r="J16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2493,10 +2821,10 @@
         <v>35</v>
       </c>
       <c r="I18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K18" t="s">
         <v>39</v>
@@ -2519,10 +2847,10 @@
         <v>35</v>
       </c>
       <c r="I19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K19" t="s">
         <v>40</v>
@@ -2545,10 +2873,10 @@
         <v>35</v>
       </c>
       <c r="I20" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K20" t="s">
         <v>41</v>
@@ -2571,10 +2899,10 @@
         <v>35</v>
       </c>
       <c r="I21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K21" t="s">
         <v>47</v>
@@ -2597,10 +2925,10 @@
         <v>35</v>
       </c>
       <c r="I22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K22" t="s">
         <v>48</v>
@@ -2623,10 +2951,10 @@
         <v>35</v>
       </c>
       <c r="I23" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K23" t="s">
         <v>49</v>
@@ -2652,10 +2980,10 @@
         <v>35</v>
       </c>
       <c r="I24" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K24" t="s">
         <v>50</v>
@@ -2681,10 +3009,10 @@
         <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K25" t="s">
         <v>51</v>
@@ -2710,10 +3038,10 @@
         <v>35</v>
       </c>
       <c r="I26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K26" t="s">
         <v>52</v>
@@ -2739,10 +3067,10 @@
         <v>35</v>
       </c>
       <c r="I27" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K27" t="s">
         <v>53</v>
@@ -2768,10 +3096,10 @@
         <v>35</v>
       </c>
       <c r="I28" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K28" t="s">
         <v>53</v>
@@ -2797,10 +3125,10 @@
         <v>35</v>
       </c>
       <c r="I29" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J29" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K29" t="s">
         <v>54</v>
@@ -2826,10 +3154,10 @@
         <v>35</v>
       </c>
       <c r="I30" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J30" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K30" t="s">
         <v>55</v>
@@ -2855,10 +3183,10 @@
         <v>35</v>
       </c>
       <c r="I31" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K31" t="s">
         <v>56</v>
@@ -2884,10 +3212,10 @@
         <v>35</v>
       </c>
       <c r="I32" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K32" t="s">
         <v>52</v>
@@ -2913,10 +3241,10 @@
         <v>35</v>
       </c>
       <c r="I33" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J33" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K33" t="s">
         <v>57</v>
@@ -2942,10 +3270,10 @@
         <v>35</v>
       </c>
       <c r="I34" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K34" t="s">
         <v>57</v>
@@ -2971,10 +3299,10 @@
         <v>35</v>
       </c>
       <c r="I35" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J35" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K35" t="s">
         <v>58</v>
@@ -2992,7 +3320,7 @@
         <v>5.6666666666666671E-3</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>113</v>
@@ -3001,10 +3329,10 @@
         <v>112</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="5" customFormat="1">
@@ -3019,7 +3347,7 @@
         <v>7.1833333333333332E-2</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>113</v>
@@ -3028,10 +3356,10 @@
         <v>112</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="5" customFormat="1">
@@ -3046,7 +3374,7 @@
         <v>0.18799999999999997</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>113</v>
@@ -3055,10 +3383,10 @@
         <v>112</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K38" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="5" customFormat="1">
@@ -3073,7 +3401,7 @@
         <v>0.27450000000000002</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>113</v>
@@ -3082,18 +3410,18 @@
         <v>112</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="5" customFormat="1">
       <c r="A40" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>108</v>
@@ -3112,18 +3440,18 @@
         <v>112</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K40" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="5" customFormat="1">
       <c r="A41" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>107</v>
@@ -3142,18 +3470,18 @@
         <v>112</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="5" customFormat="1">
       <c r="A42" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>109</v>
@@ -3172,18 +3500,18 @@
         <v>112</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="5" customFormat="1">
       <c r="A43" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>110</v>
@@ -3202,10 +3530,10 @@
         <v>112</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -3234,7 +3562,7 @@
         <v>123</v>
       </c>
       <c r="J44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K44" t="s">
         <v>130</v>
@@ -3266,7 +3594,7 @@
         <v>123</v>
       </c>
       <c r="J45" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K45" t="s">
         <v>131</v>
@@ -3298,7 +3626,7 @@
         <v>123</v>
       </c>
       <c r="J46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K46" t="s">
         <v>164</v>
@@ -3309,7 +3637,7 @@
         <v>155</v>
       </c>
       <c r="B47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C47" t="s">
         <v>163</v>
@@ -3327,7 +3655,7 @@
         <v>123</v>
       </c>
       <c r="J47" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K47" t="s">
         <v>156</v>
@@ -3338,7 +3666,7 @@
         <v>155</v>
       </c>
       <c r="B48" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C48" t="s">
         <v>159</v>
@@ -3356,7 +3684,7 @@
         <v>123</v>
       </c>
       <c r="J48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K48" t="s">
         <v>156</v>
@@ -3367,7 +3695,7 @@
         <v>155</v>
       </c>
       <c r="B49" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C49" t="s">
         <v>162</v>
@@ -3385,7 +3713,7 @@
         <v>123</v>
       </c>
       <c r="J49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K49" t="s">
         <v>156</v>
@@ -3396,7 +3724,7 @@
         <v>155</v>
       </c>
       <c r="B50" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C50" t="s">
         <v>160</v>
@@ -3414,7 +3742,7 @@
         <v>123</v>
       </c>
       <c r="J50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K50" t="s">
         <v>156</v>
@@ -3425,7 +3753,7 @@
         <v>155</v>
       </c>
       <c r="B51" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C51" t="s">
         <v>158</v>
@@ -3443,7 +3771,7 @@
         <v>123</v>
       </c>
       <c r="J51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K51" t="s">
         <v>156</v>
@@ -3454,7 +3782,7 @@
         <v>155</v>
       </c>
       <c r="B52" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C52" t="s">
         <v>161</v>
@@ -3472,370 +3800,368 @@
         <v>123</v>
       </c>
       <c r="J52" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K52" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
-      <c r="A53" t="s">
+    <row r="53" spans="1:11" s="9" customFormat="1">
+      <c r="A53" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="9">
         <v>3.07</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="9">
         <v>14.8</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G53" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="H53" t="s">
-        <v>151</v>
-      </c>
-      <c r="I53" t="s">
+      <c r="H53" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I53" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="J53" t="s">
-        <v>179</v>
-      </c>
-      <c r="K53" t="s">
+      <c r="J53" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K53" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
-      <c r="A54" t="s">
+    <row r="54" spans="1:11" s="9" customFormat="1">
+      <c r="A54" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="9">
         <v>44.3</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="9">
         <v>87.6</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G54" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="H54" t="s">
-        <v>151</v>
-      </c>
-      <c r="I54" t="s">
+      <c r="H54" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I54" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="J54" t="s">
-        <v>179</v>
-      </c>
-      <c r="K54" t="s">
+      <c r="J54" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K54" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
-      <c r="A55" t="s">
+    <row r="55" spans="1:11" s="9" customFormat="1">
+      <c r="A55" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="9">
         <v>11.25</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="9">
         <v>19.809999999999999</v>
       </c>
-      <c r="G55" t="s">
-        <v>202</v>
-      </c>
-      <c r="H55" t="s">
-        <v>151</v>
-      </c>
-      <c r="I55" t="s">
+      <c r="G55" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="H55" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I55" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="J55" t="s">
-        <v>179</v>
-      </c>
-      <c r="K55" t="s">
+      <c r="J55" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K55" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
-      <c r="A56" t="s">
+    <row r="56" spans="1:11" s="9" customFormat="1">
+      <c r="A56" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="9">
         <v>9.9</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="9">
         <v>12.5</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="H56" t="s">
-        <v>151</v>
-      </c>
-      <c r="I56" t="s">
+      <c r="H56" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I56" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="J56" t="s">
-        <v>179</v>
-      </c>
-      <c r="K56" t="s">
+      <c r="J56" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K56" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
-      <c r="A57" t="s">
+    <row r="57" spans="1:11" s="9" customFormat="1">
+      <c r="A57" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="9">
         <v>88.36</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="9">
         <v>511.1</v>
       </c>
-      <c r="G57" t="s">
+      <c r="G57" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H57" t="s">
-        <v>151</v>
-      </c>
-      <c r="I57" t="s">
+      <c r="H57" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I57" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="J57" t="s">
-        <v>179</v>
-      </c>
-      <c r="K57" t="s">
+      <c r="J57" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K57" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
-      <c r="A58" t="s">
+    <row r="58" spans="1:11" s="9" customFormat="1">
+      <c r="A58" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="9">
         <v>0.50900000000000001</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="9">
         <v>99.24</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="H58" t="s">
-        <v>151</v>
-      </c>
-      <c r="I58" t="s">
+      <c r="H58" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I58" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="J58" t="s">
-        <v>179</v>
-      </c>
-      <c r="K58" t="s">
+      <c r="J58" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K58" s="9" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
-      <c r="A59" t="s">
-        <v>166</v>
-      </c>
-      <c r="B59" s="5" t="s">
+    <row r="59" spans="1:11" s="9" customFormat="1">
+      <c r="A59" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D59" s="10">
+        <v>3</v>
+      </c>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10">
+        <v>20</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="J59" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K59" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" s="5" customFormat="1">
+      <c r="A60" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D60" s="7">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="K60" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" s="5" customFormat="1">
+      <c r="A61" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" t="s">
+        <v>186</v>
+      </c>
+      <c r="D62" s="4">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="G62" t="s">
         <v>192</v>
       </c>
-      <c r="C59" t="s">
-        <v>167</v>
-      </c>
-      <c r="D59">
-        <f>(15/119)*1000</f>
-        <v>126.05042016806722</v>
-      </c>
-      <c r="G59" t="s">
-        <v>154</v>
-      </c>
-      <c r="I59" t="s">
-        <v>144</v>
-      </c>
-      <c r="J59" t="s">
-        <v>179</v>
-      </c>
-      <c r="K59" t="s">
+      <c r="H62" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="I62" t="s">
+        <v>184</v>
+      </c>
+      <c r="J62" t="s">
+        <v>174</v>
+      </c>
+      <c r="K62" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" t="s">
+        <v>205</v>
+      </c>
+      <c r="C63" s="5" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" t="s">
-        <v>166</v>
-      </c>
-      <c r="B60" s="5" t="s">
+      <c r="D63" s="4">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="G63" t="s">
         <v>192</v>
       </c>
-      <c r="C60" t="s">
-        <v>168</v>
-      </c>
-      <c r="D60">
-        <f>(15/2822)*1000</f>
-        <v>5.3153791637136782</v>
-      </c>
-      <c r="G60" t="s">
-        <v>154</v>
-      </c>
-      <c r="I60" t="s">
-        <v>144</v>
-      </c>
-      <c r="J60" t="s">
-        <v>179</v>
-      </c>
-      <c r="K60" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" t="s">
-        <v>149</v>
-      </c>
-      <c r="B61" t="s">
-        <v>125</v>
-      </c>
-      <c r="C61" t="s">
-        <v>150</v>
-      </c>
-      <c r="D61" s="4">
-        <v>3</v>
-      </c>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4">
-        <v>20</v>
-      </c>
-      <c r="G61" t="s">
-        <v>201</v>
-      </c>
-      <c r="H61" t="s">
-        <v>151</v>
-      </c>
-      <c r="I61" t="s">
-        <v>152</v>
-      </c>
-      <c r="J61" t="s">
-        <v>178</v>
-      </c>
-      <c r="K61" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" s="5" customFormat="1">
-      <c r="A62" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D62" s="7">
-        <v>1.6E-2</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="K62" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" s="5" customFormat="1">
-      <c r="A63" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D63" s="7">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>193</v>
-      </c>
       <c r="H63" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="K63" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="I63" t="s">
+        <v>184</v>
+      </c>
+      <c r="J63" t="s">
+        <v>174</v>
+      </c>
+      <c r="K63" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" t="s">
-        <v>187</v>
-      </c>
-      <c r="C64" t="s">
-        <v>188</v>
+        <v>206</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="D64" s="4">
-        <v>0.54300000000000004</v>
+        <v>37.75</v>
       </c>
       <c r="G64" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I64" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J64" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K64" t="s">
         <v>143</v>
@@ -3846,22 +4172,22 @@
         <v>207</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D65" s="4">
-        <v>2.3999999999999998E-3</v>
+        <v>-9.98</v>
       </c>
       <c r="G65" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I65" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K65" t="s">
         <v>143</v>
@@ -3869,25 +4195,25 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" t="s">
+        <v>207</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="G66" t="s">
         <v>208</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D66" s="4">
-        <v>37.75</v>
-      </c>
-      <c r="G66" t="s">
-        <v>194</v>
-      </c>
       <c r="H66" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I66" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J66" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K66" t="s">
         <v>143</v>
@@ -3895,209 +4221,157 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67" t="s">
+        <v>186</v>
+      </c>
+      <c r="D67">
+        <v>506</v>
+      </c>
+      <c r="G67" t="s">
+        <v>193</v>
+      </c>
+      <c r="H67" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D67" s="4">
-        <v>-9.98</v>
-      </c>
-      <c r="G67" t="s">
-        <v>210</v>
-      </c>
-      <c r="H67" s="5" t="s">
-        <v>211</v>
-      </c>
       <c r="I67" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J67" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K67" t="s">
-        <v>143</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
-        <v>209</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D68" s="4">
-        <v>0.68600000000000005</v>
+        <v>124</v>
+      </c>
+      <c r="B68" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" t="s">
+        <v>242</v>
+      </c>
+      <c r="D68">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F68">
+        <v>0.65900000000000003</v>
       </c>
       <c r="G68" t="s">
+        <v>212</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="I68" t="s">
         <v>210</v>
       </c>
-      <c r="H68" s="5" t="s">
+      <c r="J68" t="s">
         <v>211</v>
       </c>
-      <c r="I68" t="s">
-        <v>186</v>
-      </c>
-      <c r="J68" t="s">
-        <v>175</v>
-      </c>
       <c r="K68" t="s">
-        <v>143</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
-        <v>189</v>
-      </c>
-      <c r="B69" t="s">
-        <v>190</v>
-      </c>
-      <c r="C69" t="s">
-        <v>188</v>
+        <v>251</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>247</v>
       </c>
       <c r="D69">
-        <v>506</v>
+        <v>32.049999999999997</v>
+      </c>
+      <c r="F69">
+        <v>111.33</v>
       </c>
       <c r="G69" t="s">
-        <v>195</v>
+        <v>250</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>211</v>
+        <v>35</v>
       </c>
       <c r="I69" t="s">
-        <v>186</v>
+        <v>246</v>
       </c>
       <c r="J69" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="K69" t="s">
-        <v>191</v>
+        <v>252</v>
       </c>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
-        <v>124</v>
-      </c>
-      <c r="B70" t="s">
-        <v>125</v>
-      </c>
-      <c r="C70" t="s">
-        <v>244</v>
+        <v>251</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>248</v>
       </c>
       <c r="D70">
-        <v>6.9000000000000006E-2</v>
+        <v>57.07</v>
       </c>
       <c r="F70">
-        <v>0.65900000000000003</v>
+        <v>176.34</v>
       </c>
       <c r="G70" t="s">
-        <v>214</v>
+        <v>250</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>151</v>
+        <v>35</v>
       </c>
       <c r="I70" t="s">
-        <v>212</v>
+        <v>246</v>
       </c>
       <c r="J70" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
       <c r="K70" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>249</v>
       </c>
       <c r="D71">
-        <v>32.049999999999997</v>
+        <v>45.82</v>
       </c>
       <c r="F71">
-        <v>111.33</v>
+        <v>95.3</v>
       </c>
       <c r="G71" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>35</v>
       </c>
       <c r="I71" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J71" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K71" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
-      <c r="A72" t="s">
-        <v>253</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="D72">
-        <v>57.07</v>
-      </c>
-      <c r="F72">
-        <v>176.34</v>
-      </c>
-      <c r="G72" t="s">
         <v>252</v>
       </c>
-      <c r="H72" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I72" t="s">
-        <v>248</v>
-      </c>
-      <c r="J72" t="s">
-        <v>181</v>
-      </c>
-      <c r="K72" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11">
-      <c r="A73" t="s">
-        <v>253</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="D73">
-        <v>45.82</v>
-      </c>
-      <c r="F73">
-        <v>95.3</v>
-      </c>
-      <c r="G73" t="s">
-        <v>252</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="I73" t="s">
-        <v>248</v>
-      </c>
-      <c r="J73" t="s">
-        <v>181</v>
-      </c>
-      <c r="K73" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11">
-      <c r="A80" s="6"/>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="6"/>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="6"/>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4309,13 +4583,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4331,10 +4605,2287 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L76"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="2" max="2" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="35.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="9" customFormat="1">
+      <c r="A2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="9">
+        <v>3.07</v>
+      </c>
+      <c r="F2" s="9">
+        <v>14.8</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="9" customFormat="1">
+      <c r="A3" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="9">
+        <v>44.3</v>
+      </c>
+      <c r="F3" s="9">
+        <v>87.6</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="9" customFormat="1">
+      <c r="A4" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="9">
+        <v>11.25</v>
+      </c>
+      <c r="F4" s="9">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="9" customFormat="1">
+      <c r="A5" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="9">
+        <v>9.9</v>
+      </c>
+      <c r="F5" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="9" customFormat="1">
+      <c r="A6" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="9">
+        <v>88.36</v>
+      </c>
+      <c r="F6" s="9">
+        <v>511.1</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="9" customFormat="1">
+      <c r="A7" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="F7" s="9">
+        <v>99.24</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="9" customFormat="1">
+      <c r="A8" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="10">
+        <v>3</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10">
+        <v>20</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11">
+        <f>L11*100</f>
+        <v>11.231724999999999</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I11" t="s">
+        <v>267</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" t="s">
+        <v>266</v>
+      </c>
+      <c r="L11">
+        <v>0.11231724999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ref="D12:D32" si="0">L12*100</f>
+        <v>11.995101</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I12" t="s">
+        <v>267</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K12" t="s">
+        <v>266</v>
+      </c>
+      <c r="L12">
+        <v>0.11995101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>11.682043999999999</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I13" t="s">
+        <v>267</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K13" t="s">
+        <v>266</v>
+      </c>
+      <c r="L13">
+        <v>0.11682044</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>11.649679000000001</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I14" t="s">
+        <v>267</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K14" t="s">
+        <v>266</v>
+      </c>
+      <c r="L14">
+        <v>0.11649679</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" t="s">
+        <v>259</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>12.526606000000001</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I15" t="s">
+        <v>267</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K15" t="s">
+        <v>266</v>
+      </c>
+      <c r="L15">
+        <v>0.12526606000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" t="s">
+        <v>249</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>12.445793</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I16" t="s">
+        <v>267</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K16" t="s">
+        <v>266</v>
+      </c>
+      <c r="L16">
+        <v>0.12445792999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" t="s">
+        <v>260</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>10.263361</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I17" t="s">
+        <v>267</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K17" t="s">
+        <v>266</v>
+      </c>
+      <c r="L17">
+        <v>0.10263361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>11.342297</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I18" t="s">
+        <v>267</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K18" t="s">
+        <v>266</v>
+      </c>
+      <c r="L18">
+        <v>0.11342297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>262</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>10.687955000000001</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I19" t="s">
+        <v>267</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K19" t="s">
+        <v>266</v>
+      </c>
+      <c r="L19">
+        <v>0.10687955</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
+        <v>263</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>9.8761329999999994</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I20" t="s">
+        <v>267</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K20" t="s">
+        <v>266</v>
+      </c>
+      <c r="L20">
+        <v>9.8761329999999994E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" t="s">
+        <v>264</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>11.595305999999999</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I21" t="s">
+        <v>267</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K21" t="s">
+        <v>266</v>
+      </c>
+      <c r="L21">
+        <v>0.11595306</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>60.758650000000003</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I22" t="s">
+        <v>267</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K22" t="s">
+        <v>266</v>
+      </c>
+      <c r="L22">
+        <v>0.60758650000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" t="s">
+        <v>258</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>46.234780000000001</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" t="s">
+        <v>267</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K23" t="s">
+        <v>266</v>
+      </c>
+      <c r="L23">
+        <v>0.46234779999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>46.312370000000001</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I24" t="s">
+        <v>267</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K24" t="s">
+        <v>266</v>
+      </c>
+      <c r="L24">
+        <v>0.46312370000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>87.570440000000005</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I25" t="s">
+        <v>267</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K25" t="s">
+        <v>266</v>
+      </c>
+      <c r="L25">
+        <v>0.87570440000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>259</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>41.470140000000001</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I26" t="s">
+        <v>267</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K26" t="s">
+        <v>266</v>
+      </c>
+      <c r="L26">
+        <v>0.4147014</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" t="s">
+        <v>249</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>80.407879999999992</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I27" t="s">
+        <v>267</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K27" t="s">
+        <v>266</v>
+      </c>
+      <c r="L27">
+        <v>0.80407879999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>68.397819999999996</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I28" t="s">
+        <v>267</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K28" t="s">
+        <v>266</v>
+      </c>
+      <c r="L28">
+        <v>0.68397819999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" t="s">
+        <v>261</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>85.797229999999999</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" t="s">
+        <v>267</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K29" t="s">
+        <v>266</v>
+      </c>
+      <c r="L29">
+        <v>0.85797230000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" t="s">
+        <v>262</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>44.345829999999999</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I30" t="s">
+        <v>267</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K30" t="s">
+        <v>266</v>
+      </c>
+      <c r="L30">
+        <v>0.44345830000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" t="s">
+        <v>263</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>63.403269999999999</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I31" t="s">
+        <v>267</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K31" t="s">
+        <v>266</v>
+      </c>
+      <c r="L31">
+        <v>0.6340327</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" t="s">
+        <v>264</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>74.21199</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I32" t="s">
+        <v>267</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K32" t="s">
+        <v>266</v>
+      </c>
+      <c r="L32">
+        <v>0.74211990000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C33" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33">
+        <v>11.25098</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I33" t="s">
+        <v>267</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K33" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" t="s">
+        <v>258</v>
+      </c>
+      <c r="D34">
+        <v>18.074259999999999</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I34" t="s">
+        <v>267</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K34" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" t="s">
+        <v>247</v>
+      </c>
+      <c r="D35">
+        <v>12.540480000000001</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I35" t="s">
+        <v>267</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K35" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36">
+        <v>13.586080000000001</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I36" t="s">
+        <v>267</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K36" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" t="s">
+        <v>259</v>
+      </c>
+      <c r="D37">
+        <v>11.46134</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I37" t="s">
+        <v>267</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K37" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" t="s">
+        <v>249</v>
+      </c>
+      <c r="D38">
+        <v>12.55148</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I38" t="s">
+        <v>267</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K38" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" t="s">
+        <v>260</v>
+      </c>
+      <c r="D39">
+        <v>12.971780000000001</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I39" t="s">
+        <v>267</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K39" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" t="s">
+        <v>261</v>
+      </c>
+      <c r="D40">
+        <v>14.30672</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I40" t="s">
+        <v>267</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K40" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" t="s">
+        <v>262</v>
+      </c>
+      <c r="D41">
+        <v>14.285640000000001</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I41" t="s">
+        <v>267</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K41" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" t="s">
+        <v>263</v>
+      </c>
+      <c r="D42">
+        <v>13.65856</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I42" t="s">
+        <v>267</v>
+      </c>
+      <c r="J42" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K42" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" t="s">
+        <v>264</v>
+      </c>
+      <c r="D43">
+        <v>19.810860000000002</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I43" t="s">
+        <v>267</v>
+      </c>
+      <c r="J43" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K43" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44">
+        <v>5.3061800000000003</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I44" t="s">
+        <v>267</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K44" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C45" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45">
+        <v>10.199859999999999</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I45" t="s">
+        <v>267</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K45" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" t="s">
+        <v>247</v>
+      </c>
+      <c r="D46">
+        <v>4.2013199999999999</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I46" t="s">
+        <v>267</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K46" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" t="s">
+        <v>168</v>
+      </c>
+      <c r="D47">
+        <v>6.3543000000000003</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I47" t="s">
+        <v>267</v>
+      </c>
+      <c r="J47" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K47" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" t="s">
+        <v>259</v>
+      </c>
+      <c r="D48">
+        <v>3.0649999999999999</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I48" t="s">
+        <v>267</v>
+      </c>
+      <c r="J48" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K48" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" t="s">
+        <v>249</v>
+      </c>
+      <c r="D49">
+        <v>7.4528600000000003</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I49" t="s">
+        <v>267</v>
+      </c>
+      <c r="J49" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K49" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C50" t="s">
+        <v>260</v>
+      </c>
+      <c r="D50">
+        <v>3.7664200000000001</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I50" t="s">
+        <v>267</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K50" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C51" t="s">
+        <v>261</v>
+      </c>
+      <c r="D51">
+        <v>14.392060000000001</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I51" t="s">
+        <v>267</v>
+      </c>
+      <c r="J51" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K51" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C52" t="s">
+        <v>262</v>
+      </c>
+      <c r="D52">
+        <v>6.9241799999999998</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I52" t="s">
+        <v>267</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K52" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" t="s">
+        <v>263</v>
+      </c>
+      <c r="D53">
+        <v>3.5022199999999999</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I53" t="s">
+        <v>267</v>
+      </c>
+      <c r="J53" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K53" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C54" t="s">
+        <v>264</v>
+      </c>
+      <c r="D54">
+        <v>14.835979999999999</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I54" t="s">
+        <v>267</v>
+      </c>
+      <c r="J54" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K54" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C55" t="s">
+        <v>167</v>
+      </c>
+      <c r="D55">
+        <f>L55*1000</f>
+        <v>6.726</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H55" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I55" t="s">
+        <v>267</v>
+      </c>
+      <c r="J55" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K55" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L55">
+        <v>6.7260000000000002E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B56" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C56" t="s">
+        <v>258</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ref="D56:D65" si="1">L56*1000</f>
+        <v>2.0617999999999999</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I56" t="s">
+        <v>267</v>
+      </c>
+      <c r="J56" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K56" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L56">
+        <v>2.0617999999999999E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C57" t="s">
+        <v>247</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>2.2239999999999998</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I57" t="s">
+        <v>267</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L57">
+        <v>2.2239999999999998E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C58" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>0.28350000000000003</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I58" t="s">
+        <v>267</v>
+      </c>
+      <c r="J58" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K58" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L58">
+        <v>2.8350000000000001E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B59" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C59" t="s">
+        <v>259</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>0.32939999999999997</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I59" t="s">
+        <v>267</v>
+      </c>
+      <c r="J59" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K59" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L59">
+        <v>3.2939999999999998E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" t="s">
+        <v>249</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>4.0733000000000006</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I60" t="s">
+        <v>267</v>
+      </c>
+      <c r="J60" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K60" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L60">
+        <v>4.0733000000000002E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B61" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C61" t="s">
+        <v>260</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>0.47839999999999999</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I61" t="s">
+        <v>267</v>
+      </c>
+      <c r="J61" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K61" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L61">
+        <v>4.7839999999999997E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" t="s">
+        <v>261</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>1.008</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H62" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I62" t="s">
+        <v>267</v>
+      </c>
+      <c r="J62" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K62" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L62">
+        <v>1.008E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" t="s">
+        <v>262</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>1.478</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I63" t="s">
+        <v>267</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K63" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L63">
+        <v>1.4779999999999999E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B64" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" t="s">
+        <v>263</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I64" t="s">
+        <v>267</v>
+      </c>
+      <c r="J64" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K64" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L64">
+        <v>4.28E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C65" t="s">
+        <v>264</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>0.34789999999999999</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="I65" t="s">
+        <v>267</v>
+      </c>
+      <c r="J65" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K65" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="L65">
+        <v>3.479E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B66" s="12"/>
+      <c r="C66" t="s">
+        <v>167</v>
+      </c>
+      <c r="D66">
+        <v>3.4847034999999998E-2</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I66" t="s">
+        <v>267</v>
+      </c>
+      <c r="K66" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B67" s="11"/>
+      <c r="C67" t="s">
+        <v>258</v>
+      </c>
+      <c r="D67">
+        <v>4.5753848999999999E-2</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I67" t="s">
+        <v>267</v>
+      </c>
+      <c r="K67" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="B68" s="11"/>
+      <c r="C68" t="s">
+        <v>247</v>
+      </c>
+      <c r="D68">
+        <v>0.14552325399999999</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H68" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I68" t="s">
+        <v>267</v>
+      </c>
+      <c r="K68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C69" t="s">
+        <v>168</v>
+      </c>
+      <c r="D69">
+        <v>6.1591535000000003E-2</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H69" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I69" t="s">
+        <v>267</v>
+      </c>
+      <c r="K69" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C70" t="s">
+        <v>259</v>
+      </c>
+      <c r="D70">
+        <v>0.34550171800000001</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H70" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I70" t="s">
+        <v>267</v>
+      </c>
+      <c r="K70" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C71" t="s">
+        <v>249</v>
+      </c>
+      <c r="D71">
+        <v>1.7112506999999999E-2</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I71" t="s">
+        <v>267</v>
+      </c>
+      <c r="K71" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C72" t="s">
+        <v>260</v>
+      </c>
+      <c r="D72">
+        <v>1.8518657000000001E-2</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H72" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I72" t="s">
+        <v>267</v>
+      </c>
+      <c r="K72" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
+      <c r="A73" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C73" t="s">
+        <v>261</v>
+      </c>
+      <c r="D73">
+        <v>1.5732459999999999E-3</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H73" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I73" t="s">
+        <v>267</v>
+      </c>
+      <c r="K73" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C74" t="s">
+        <v>262</v>
+      </c>
+      <c r="D74">
+        <v>0.12609704199999999</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I74" t="s">
+        <v>267</v>
+      </c>
+      <c r="K74" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
+      <c r="A75" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C75" t="s">
+        <v>263</v>
+      </c>
+      <c r="D75">
+        <v>0.19160534300000001</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H75" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I75" t="s">
+        <v>267</v>
+      </c>
+      <c r="K75" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
+      <c r="A76" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="C76" t="s">
+        <v>264</v>
+      </c>
+      <c r="D76">
+        <v>1.1875814E-2</v>
+      </c>
+      <c r="G76" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="H76" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="I76" t="s">
+        <v>267</v>
+      </c>
+      <c r="K76" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30:G56"/>
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4344,7 +6895,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B1" t="s">
         <v>125</v>
@@ -4352,7 +6903,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B2">
         <v>0.32</v>
@@ -4360,7 +6911,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B3">
         <v>0.183</v>
@@ -4368,7 +6919,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B4">
         <v>0.38700000000000001</v>
@@ -4376,7 +6927,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B5">
         <v>0.65900000000000003</v>
@@ -4384,7 +6935,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B6">
         <v>0.14399999999999999</v>
@@ -4392,7 +6943,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B7">
         <v>0.21299999999999999</v>
@@ -4400,7 +6951,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B8">
         <v>0.45800000000000002</v>
@@ -4408,7 +6959,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B9">
         <v>0.28799999999999998</v>
@@ -4416,7 +6967,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B10">
         <v>0.24199999999999999</v>
@@ -4424,7 +6975,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="8" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B11">
         <v>0.51500000000000001</v>
@@ -4432,7 +6983,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="8" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B12">
         <v>0.26600000000000001</v>
@@ -4440,7 +6991,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B13">
         <v>0.22</v>
@@ -4448,7 +6999,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B14">
         <v>0.29699999999999999</v>
@@ -4456,7 +7007,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B15">
         <v>0.161</v>
@@ -4464,7 +7015,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B16">
         <v>0.18099999999999999</v>
@@ -4472,7 +7023,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B17">
         <v>0.10199999999999999</v>
@@ -4480,7 +7031,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B18">
         <v>0.38100000000000001</v>
@@ -4488,7 +7039,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B19">
         <v>0.32100000000000001</v>
@@ -4496,7 +7047,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B20">
         <v>0.22600000000000001</v>
@@ -4504,7 +7055,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B21">
         <v>0.38400000000000001</v>
@@ -4512,7 +7063,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B22">
         <v>0.52100000000000002</v>
@@ -4520,7 +7071,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B23">
         <v>6.9000000000000006E-2</v>
@@ -4528,7 +7079,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B24">
         <v>0.13300000000000001</v>
@@ -4536,7 +7087,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="8" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B25">
         <v>6.9000000000000006E-2</v>
@@ -4544,7 +7095,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B26">
         <v>0.115</v>
@@ -4552,7 +7103,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="8" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B27">
         <v>0.17899999999999999</v>
@@ -4560,7 +7111,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B28">
         <v>0.44</v>
@@ -4580,7 +7131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>